<commit_message>
Untested Binary Search for previous seasons
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,31 +434,107 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>('Samira', 360)</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Sinvu#NA1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>('Caitlyn', 51)</t>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>winRate</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>avgCS</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>GPM</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>KP</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>avgDPM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>avgAbusage</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>visionScore</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>numGames</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>{'KDA': (4.666666666666667, 6.666666666666667, 4.333333333333333), 'winRate': 0.0, 'avgCS': 5.126959735551346, 'GPM': 349.3391168980931, 'KP': 0.3914398064125832, 'avgDPM': 399.52275566741474, 'avgAbusage': 141.0, 'visionScore': 14.666666666666666, 'numGames': 3}</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>{'KDA': (0.0, 2.0, 4.0), 'winRate': 1.0, 'avgCS': 5.057223897771736, 'GPM': 317.7436714810554, 'KP': 0.21052631578947367, 'avgDPM': 326.1735909902009, 'avgAbusage': 79.0, 'visionScore': 13.0, 'numGames': 1}</t>
-        </is>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Yorick</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" t="n">
+        <v>427</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>712</v>
+      </c>
+      <c r="J2" t="n">
+        <v>250</v>
+      </c>
+      <c r="K2" t="n">
+        <v>17</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized searching algorithm for previous games and implemented TOCSV method.
</commit_message>
<xml_diff>
--- a/excel/output.xlsx
+++ b/excel/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,26 +498,26 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Yorick</t>
+          <t>Thresh</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>427</v>
+        <v>285</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -525,16 +525,226 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>712</v>
+        <v>264</v>
       </c>
       <c r="J2" t="n">
-        <v>250</v>
+        <v>89</v>
       </c>
       <c r="K2" t="n">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="L2" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bard</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>220</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>217</v>
+      </c>
+      <c r="J3" t="n">
+        <v>84</v>
+      </c>
+      <c r="K3" t="n">
+        <v>23</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Sion</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G4" t="n">
+        <v>400</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>640</v>
+      </c>
+      <c r="J4" t="n">
+        <v>185</v>
+      </c>
+      <c r="K4" t="n">
+        <v>14</v>
+      </c>
+      <c r="L4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Yorick</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" t="n">
+        <v>440</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>643</v>
+      </c>
+      <c r="J5" t="n">
+        <v>216</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15</v>
+      </c>
+      <c r="L5" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Yone</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" t="n">
+        <v>371</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>707</v>
+      </c>
+      <c r="J6" t="n">
+        <v>292</v>
+      </c>
+      <c r="K6" t="n">
+        <v>11</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Ornn</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" t="n">
+        <v>366</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>659</v>
+      </c>
+      <c r="J7" t="n">
+        <v>218</v>
+      </c>
+      <c r="K7" t="n">
+        <v>19</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>